<commit_message>
ALARM CLASSIFICATION BUG FIXED
</commit_message>
<xml_diff>
--- a/1toolConverter_local/parametros_convertidos.xlsx
+++ b/1toolConverter_local/parametros_convertidos.xlsx
@@ -17656,7 +17656,7 @@
       </c>
       <c r="E176" t="inlineStr">
         <is>
-          <t>CONFIG_PARAMETER</t>
+          <t>ALARM</t>
         </is>
       </c>
       <c r="F176" t="inlineStr"/>
@@ -17666,13 +17666,13 @@
         </is>
       </c>
       <c r="H176" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I176" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J176" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="K176" t="n">
         <v>1</v>
@@ -35394,7 +35394,7 @@
       </c>
       <c r="E357" t="inlineStr">
         <is>
-          <t>DIGITAL_INPUT</t>
+          <t>ALARM</t>
         </is>
       </c>
       <c r="F357" t="inlineStr"/>
@@ -35404,7 +35404,7 @@
         </is>
       </c>
       <c r="H357" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I357" t="n">
         <v>4</v>
@@ -35590,7 +35590,7 @@
       </c>
       <c r="E359" t="inlineStr">
         <is>
-          <t>COMMAND</t>
+          <t>ALARM</t>
         </is>
       </c>
       <c r="F359" t="inlineStr"/>
@@ -35600,13 +35600,13 @@
         </is>
       </c>
       <c r="H359" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I359" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J359" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="K359" t="n">
         <v>0</v>
@@ -37938,7 +37938,7 @@
       <c r="D383" t="inlineStr"/>
       <c r="E383" t="inlineStr">
         <is>
-          <t>DIGITAL_INPUT</t>
+          <t>ALARM</t>
         </is>
       </c>
       <c r="F383" t="inlineStr"/>
@@ -37948,7 +37948,7 @@
         </is>
       </c>
       <c r="H383" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I383" t="n">
         <v>4</v>
@@ -40188,7 +40188,7 @@
       <c r="D406" t="inlineStr"/>
       <c r="E406" t="inlineStr">
         <is>
-          <t>DIGITAL_INPUT</t>
+          <t>ALARM</t>
         </is>
       </c>
       <c r="F406" t="inlineStr"/>
@@ -40198,7 +40198,7 @@
         </is>
       </c>
       <c r="H406" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I406" t="n">
         <v>4</v>
@@ -40286,7 +40286,7 @@
       </c>
       <c r="E407" t="inlineStr">
         <is>
-          <t>DIGITAL_INPUT</t>
+          <t>ALARM</t>
         </is>
       </c>
       <c r="F407" t="inlineStr"/>
@@ -40296,7 +40296,7 @@
         </is>
       </c>
       <c r="H407" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I407" t="n">
         <v>4</v>
@@ -40384,7 +40384,7 @@
       </c>
       <c r="E408" t="inlineStr">
         <is>
-          <t>DIGITAL_INPUT</t>
+          <t>ALARM</t>
         </is>
       </c>
       <c r="F408" t="inlineStr"/>
@@ -40394,7 +40394,7 @@
         </is>
       </c>
       <c r="H408" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I408" t="n">
         <v>4</v>
@@ -40482,7 +40482,7 @@
       </c>
       <c r="E409" t="inlineStr">
         <is>
-          <t>DIGITAL_INPUT</t>
+          <t>ALARM</t>
         </is>
       </c>
       <c r="F409" t="inlineStr"/>
@@ -40492,7 +40492,7 @@
         </is>
       </c>
       <c r="H409" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I409" t="n">
         <v>4</v>
@@ -40580,7 +40580,7 @@
       </c>
       <c r="E410" t="inlineStr">
         <is>
-          <t>DIGITAL_INPUT</t>
+          <t>ALARM</t>
         </is>
       </c>
       <c r="F410" t="inlineStr"/>
@@ -40590,7 +40590,7 @@
         </is>
       </c>
       <c r="H410" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I410" t="n">
         <v>4</v>
@@ -40678,7 +40678,7 @@
       </c>
       <c r="E411" t="inlineStr">
         <is>
-          <t>DIGITAL_INPUT</t>
+          <t>ALARM</t>
         </is>
       </c>
       <c r="F411" t="inlineStr"/>
@@ -40688,7 +40688,7 @@
         </is>
       </c>
       <c r="H411" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I411" t="n">
         <v>4</v>
@@ -40776,7 +40776,7 @@
       </c>
       <c r="E412" t="inlineStr">
         <is>
-          <t>DIGITAL_INPUT</t>
+          <t>ALARM</t>
         </is>
       </c>
       <c r="F412" t="inlineStr"/>
@@ -40786,7 +40786,7 @@
         </is>
       </c>
       <c r="H412" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I412" t="n">
         <v>4</v>
@@ -42438,7 +42438,7 @@
       <c r="D429" t="inlineStr"/>
       <c r="E429" t="inlineStr">
         <is>
-          <t>DIGITAL_INPUT</t>
+          <t>ALARM</t>
         </is>
       </c>
       <c r="F429" t="inlineStr"/>
@@ -42448,7 +42448,7 @@
         </is>
       </c>
       <c r="H429" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I429" t="n">
         <v>4</v>
@@ -42536,7 +42536,7 @@
       </c>
       <c r="E430" t="inlineStr">
         <is>
-          <t>DIGITAL_INPUT</t>
+          <t>ALARM</t>
         </is>
       </c>
       <c r="F430" t="inlineStr"/>
@@ -42546,7 +42546,7 @@
         </is>
       </c>
       <c r="H430" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I430" t="n">
         <v>4</v>
@@ -42634,7 +42634,7 @@
       </c>
       <c r="E431" t="inlineStr">
         <is>
-          <t>DIGITAL_INPUT</t>
+          <t>ALARM</t>
         </is>
       </c>
       <c r="F431" t="inlineStr"/>
@@ -42644,7 +42644,7 @@
         </is>
       </c>
       <c r="H431" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I431" t="n">
         <v>4</v>
@@ -42732,7 +42732,7 @@
       </c>
       <c r="E432" t="inlineStr">
         <is>
-          <t>DIGITAL_INPUT</t>
+          <t>ALARM</t>
         </is>
       </c>
       <c r="F432" t="inlineStr"/>
@@ -42742,7 +42742,7 @@
         </is>
       </c>
       <c r="H432" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I432" t="n">
         <v>4</v>
@@ -42830,7 +42830,7 @@
       </c>
       <c r="E433" t="inlineStr">
         <is>
-          <t>DIGITAL_INPUT</t>
+          <t>ALARM</t>
         </is>
       </c>
       <c r="F433" t="inlineStr"/>
@@ -42840,7 +42840,7 @@
         </is>
       </c>
       <c r="H433" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I433" t="n">
         <v>4</v>
@@ -42928,7 +42928,7 @@
       </c>
       <c r="E434" t="inlineStr">
         <is>
-          <t>DIGITAL_INPUT</t>
+          <t>ALARM</t>
         </is>
       </c>
       <c r="F434" t="inlineStr"/>
@@ -42938,7 +42938,7 @@
         </is>
       </c>
       <c r="H434" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I434" t="n">
         <v>4</v>
@@ -43026,7 +43026,7 @@
       </c>
       <c r="E435" t="inlineStr">
         <is>
-          <t>DIGITAL_INPUT</t>
+          <t>ALARM</t>
         </is>
       </c>
       <c r="F435" t="inlineStr"/>
@@ -43036,7 +43036,7 @@
         </is>
       </c>
       <c r="H435" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I435" t="n">
         <v>4</v>
@@ -44688,7 +44688,7 @@
       <c r="D452" t="inlineStr"/>
       <c r="E452" t="inlineStr">
         <is>
-          <t>DIGITAL_INPUT</t>
+          <t>ALARM</t>
         </is>
       </c>
       <c r="F452" t="inlineStr"/>
@@ -44698,7 +44698,7 @@
         </is>
       </c>
       <c r="H452" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I452" t="n">
         <v>4</v>
@@ -44786,7 +44786,7 @@
       </c>
       <c r="E453" t="inlineStr">
         <is>
-          <t>DIGITAL_INPUT</t>
+          <t>ALARM</t>
         </is>
       </c>
       <c r="F453" t="inlineStr"/>
@@ -44796,7 +44796,7 @@
         </is>
       </c>
       <c r="H453" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I453" t="n">
         <v>4</v>
@@ -44884,7 +44884,7 @@
       </c>
       <c r="E454" t="inlineStr">
         <is>
-          <t>DIGITAL_INPUT</t>
+          <t>ALARM</t>
         </is>
       </c>
       <c r="F454" t="inlineStr"/>
@@ -44894,7 +44894,7 @@
         </is>
       </c>
       <c r="H454" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I454" t="n">
         <v>4</v>
@@ -44982,7 +44982,7 @@
       </c>
       <c r="E455" t="inlineStr">
         <is>
-          <t>DIGITAL_INPUT</t>
+          <t>ALARM</t>
         </is>
       </c>
       <c r="F455" t="inlineStr"/>
@@ -44992,7 +44992,7 @@
         </is>
       </c>
       <c r="H455" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I455" t="n">
         <v>4</v>
@@ -45080,7 +45080,7 @@
       </c>
       <c r="E456" t="inlineStr">
         <is>
-          <t>DIGITAL_INPUT</t>
+          <t>ALARM</t>
         </is>
       </c>
       <c r="F456" t="inlineStr"/>
@@ -45090,7 +45090,7 @@
         </is>
       </c>
       <c r="H456" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I456" t="n">
         <v>4</v>
@@ -45178,7 +45178,7 @@
       </c>
       <c r="E457" t="inlineStr">
         <is>
-          <t>DIGITAL_INPUT</t>
+          <t>ALARM</t>
         </is>
       </c>
       <c r="F457" t="inlineStr"/>
@@ -45188,7 +45188,7 @@
         </is>
       </c>
       <c r="H457" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I457" t="n">
         <v>4</v>
@@ -45276,7 +45276,7 @@
       </c>
       <c r="E458" t="inlineStr">
         <is>
-          <t>DIGITAL_INPUT</t>
+          <t>ALARM</t>
         </is>
       </c>
       <c r="F458" t="inlineStr"/>
@@ -45286,7 +45286,7 @@
         </is>
       </c>
       <c r="H458" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I458" t="n">
         <v>4</v>
@@ -46938,7 +46938,7 @@
       <c r="D475" t="inlineStr"/>
       <c r="E475" t="inlineStr">
         <is>
-          <t>DIGITAL_INPUT</t>
+          <t>ALARM</t>
         </is>
       </c>
       <c r="F475" t="inlineStr"/>
@@ -46948,7 +46948,7 @@
         </is>
       </c>
       <c r="H475" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I475" t="n">
         <v>4</v>
@@ -47036,7 +47036,7 @@
       </c>
       <c r="E476" t="inlineStr">
         <is>
-          <t>DIGITAL_INPUT</t>
+          <t>ALARM</t>
         </is>
       </c>
       <c r="F476" t="inlineStr"/>
@@ -47046,7 +47046,7 @@
         </is>
       </c>
       <c r="H476" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I476" t="n">
         <v>4</v>
@@ -47134,7 +47134,7 @@
       </c>
       <c r="E477" t="inlineStr">
         <is>
-          <t>DIGITAL_INPUT</t>
+          <t>ALARM</t>
         </is>
       </c>
       <c r="F477" t="inlineStr"/>
@@ -47144,7 +47144,7 @@
         </is>
       </c>
       <c r="H477" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I477" t="n">
         <v>4</v>
@@ -47232,7 +47232,7 @@
       </c>
       <c r="E478" t="inlineStr">
         <is>
-          <t>DIGITAL_INPUT</t>
+          <t>ALARM</t>
         </is>
       </c>
       <c r="F478" t="inlineStr"/>
@@ -47242,7 +47242,7 @@
         </is>
       </c>
       <c r="H478" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I478" t="n">
         <v>4</v>
@@ -47330,7 +47330,7 @@
       </c>
       <c r="E479" t="inlineStr">
         <is>
-          <t>DIGITAL_INPUT</t>
+          <t>ALARM</t>
         </is>
       </c>
       <c r="F479" t="inlineStr"/>
@@ -47340,7 +47340,7 @@
         </is>
       </c>
       <c r="H479" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I479" t="n">
         <v>4</v>
@@ -47428,7 +47428,7 @@
       </c>
       <c r="E480" t="inlineStr">
         <is>
-          <t>DIGITAL_INPUT</t>
+          <t>ALARM</t>
         </is>
       </c>
       <c r="F480" t="inlineStr"/>
@@ -47438,7 +47438,7 @@
         </is>
       </c>
       <c r="H480" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I480" t="n">
         <v>4</v>
@@ -47526,7 +47526,7 @@
       </c>
       <c r="E481" t="inlineStr">
         <is>
-          <t>DIGITAL_INPUT</t>
+          <t>ALARM</t>
         </is>
       </c>
       <c r="F481" t="inlineStr"/>
@@ -47536,7 +47536,7 @@
         </is>
       </c>
       <c r="H481" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I481" t="n">
         <v>4</v>
@@ -49188,7 +49188,7 @@
       <c r="D498" t="inlineStr"/>
       <c r="E498" t="inlineStr">
         <is>
-          <t>DIGITAL_INPUT</t>
+          <t>ALARM</t>
         </is>
       </c>
       <c r="F498" t="inlineStr"/>
@@ -49198,7 +49198,7 @@
         </is>
       </c>
       <c r="H498" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I498" t="n">
         <v>4</v>
@@ -49286,7 +49286,7 @@
       </c>
       <c r="E499" t="inlineStr">
         <is>
-          <t>DIGITAL_INPUT</t>
+          <t>ALARM</t>
         </is>
       </c>
       <c r="F499" t="inlineStr"/>
@@ -49296,7 +49296,7 @@
         </is>
       </c>
       <c r="H499" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I499" t="n">
         <v>4</v>
@@ -49384,7 +49384,7 @@
       </c>
       <c r="E500" t="inlineStr">
         <is>
-          <t>DIGITAL_INPUT</t>
+          <t>ALARM</t>
         </is>
       </c>
       <c r="F500" t="inlineStr"/>
@@ -49394,7 +49394,7 @@
         </is>
       </c>
       <c r="H500" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I500" t="n">
         <v>4</v>
@@ -49482,7 +49482,7 @@
       </c>
       <c r="E501" t="inlineStr">
         <is>
-          <t>DIGITAL_INPUT</t>
+          <t>ALARM</t>
         </is>
       </c>
       <c r="F501" t="inlineStr"/>
@@ -49492,7 +49492,7 @@
         </is>
       </c>
       <c r="H501" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I501" t="n">
         <v>4</v>
@@ -49580,7 +49580,7 @@
       </c>
       <c r="E502" t="inlineStr">
         <is>
-          <t>DIGITAL_INPUT</t>
+          <t>ALARM</t>
         </is>
       </c>
       <c r="F502" t="inlineStr"/>
@@ -49590,7 +49590,7 @@
         </is>
       </c>
       <c r="H502" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I502" t="n">
         <v>4</v>
@@ -49678,7 +49678,7 @@
       </c>
       <c r="E503" t="inlineStr">
         <is>
-          <t>DIGITAL_INPUT</t>
+          <t>ALARM</t>
         </is>
       </c>
       <c r="F503" t="inlineStr"/>
@@ -49688,7 +49688,7 @@
         </is>
       </c>
       <c r="H503" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I503" t="n">
         <v>4</v>
@@ -49776,7 +49776,7 @@
       </c>
       <c r="E504" t="inlineStr">
         <is>
-          <t>DIGITAL_INPUT</t>
+          <t>ALARM</t>
         </is>
       </c>
       <c r="F504" t="inlineStr"/>
@@ -49786,7 +49786,7 @@
         </is>
       </c>
       <c r="H504" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I504" t="n">
         <v>4</v>
@@ -51438,7 +51438,7 @@
       <c r="D521" t="inlineStr"/>
       <c r="E521" t="inlineStr">
         <is>
-          <t>DIGITAL_INPUT</t>
+          <t>ALARM</t>
         </is>
       </c>
       <c r="F521" t="inlineStr"/>
@@ -51448,7 +51448,7 @@
         </is>
       </c>
       <c r="H521" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I521" t="n">
         <v>4</v>
@@ -51536,7 +51536,7 @@
       </c>
       <c r="E522" t="inlineStr">
         <is>
-          <t>DIGITAL_INPUT</t>
+          <t>ALARM</t>
         </is>
       </c>
       <c r="F522" t="inlineStr"/>
@@ -51546,7 +51546,7 @@
         </is>
       </c>
       <c r="H522" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I522" t="n">
         <v>4</v>
@@ -51634,7 +51634,7 @@
       </c>
       <c r="E523" t="inlineStr">
         <is>
-          <t>DIGITAL_INPUT</t>
+          <t>ALARM</t>
         </is>
       </c>
       <c r="F523" t="inlineStr"/>
@@ -51644,7 +51644,7 @@
         </is>
       </c>
       <c r="H523" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I523" t="n">
         <v>4</v>
@@ -51732,7 +51732,7 @@
       </c>
       <c r="E524" t="inlineStr">
         <is>
-          <t>DIGITAL_INPUT</t>
+          <t>ALARM</t>
         </is>
       </c>
       <c r="F524" t="inlineStr"/>
@@ -51742,7 +51742,7 @@
         </is>
       </c>
       <c r="H524" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I524" t="n">
         <v>4</v>
@@ -51830,7 +51830,7 @@
       </c>
       <c r="E525" t="inlineStr">
         <is>
-          <t>DIGITAL_INPUT</t>
+          <t>ALARM</t>
         </is>
       </c>
       <c r="F525" t="inlineStr"/>
@@ -51840,7 +51840,7 @@
         </is>
       </c>
       <c r="H525" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I525" t="n">
         <v>4</v>
@@ -51928,7 +51928,7 @@
       </c>
       <c r="E526" t="inlineStr">
         <is>
-          <t>DIGITAL_INPUT</t>
+          <t>ALARM</t>
         </is>
       </c>
       <c r="F526" t="inlineStr"/>
@@ -51938,7 +51938,7 @@
         </is>
       </c>
       <c r="H526" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I526" t="n">
         <v>4</v>
@@ -52026,7 +52026,7 @@
       </c>
       <c r="E527" t="inlineStr">
         <is>
-          <t>DIGITAL_INPUT</t>
+          <t>ALARM</t>
         </is>
       </c>
       <c r="F527" t="inlineStr"/>
@@ -52036,7 +52036,7 @@
         </is>
       </c>
       <c r="H527" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I527" t="n">
         <v>4</v>
@@ -53688,7 +53688,7 @@
       <c r="D544" t="inlineStr"/>
       <c r="E544" t="inlineStr">
         <is>
-          <t>DIGITAL_INPUT</t>
+          <t>ALARM</t>
         </is>
       </c>
       <c r="F544" t="inlineStr"/>
@@ -53698,7 +53698,7 @@
         </is>
       </c>
       <c r="H544" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I544" t="n">
         <v>4</v>
@@ -53786,7 +53786,7 @@
       </c>
       <c r="E545" t="inlineStr">
         <is>
-          <t>DIGITAL_INPUT</t>
+          <t>ALARM</t>
         </is>
       </c>
       <c r="F545" t="inlineStr"/>
@@ -53796,7 +53796,7 @@
         </is>
       </c>
       <c r="H545" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I545" t="n">
         <v>4</v>
@@ -53884,7 +53884,7 @@
       </c>
       <c r="E546" t="inlineStr">
         <is>
-          <t>DIGITAL_INPUT</t>
+          <t>ALARM</t>
         </is>
       </c>
       <c r="F546" t="inlineStr"/>
@@ -53894,7 +53894,7 @@
         </is>
       </c>
       <c r="H546" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I546" t="n">
         <v>4</v>
@@ -53982,7 +53982,7 @@
       </c>
       <c r="E547" t="inlineStr">
         <is>
-          <t>DIGITAL_INPUT</t>
+          <t>ALARM</t>
         </is>
       </c>
       <c r="F547" t="inlineStr"/>
@@ -53992,7 +53992,7 @@
         </is>
       </c>
       <c r="H547" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I547" t="n">
         <v>4</v>
@@ -54080,7 +54080,7 @@
       </c>
       <c r="E548" t="inlineStr">
         <is>
-          <t>DIGITAL_INPUT</t>
+          <t>ALARM</t>
         </is>
       </c>
       <c r="F548" t="inlineStr"/>
@@ -54090,7 +54090,7 @@
         </is>
       </c>
       <c r="H548" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I548" t="n">
         <v>4</v>
@@ -54178,7 +54178,7 @@
       </c>
       <c r="E549" t="inlineStr">
         <is>
-          <t>DIGITAL_INPUT</t>
+          <t>ALARM</t>
         </is>
       </c>
       <c r="F549" t="inlineStr"/>
@@ -54188,7 +54188,7 @@
         </is>
       </c>
       <c r="H549" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I549" t="n">
         <v>4</v>
@@ -54276,7 +54276,7 @@
       </c>
       <c r="E550" t="inlineStr">
         <is>
-          <t>DIGITAL_INPUT</t>
+          <t>ALARM</t>
         </is>
       </c>
       <c r="F550" t="inlineStr"/>
@@ -54286,7 +54286,7 @@
         </is>
       </c>
       <c r="H550" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I550" t="n">
         <v>4</v>

</xml_diff>